<commit_message>
Updated hyperlink, shave 50% off the per-board price by changing 2-pin terminal block suppliers.
</commit_message>
<xml_diff>
--- a/LED_Matrix_PCB/BOM.xlsx
+++ b/LED_Matrix_PCB/BOM.xlsx
@@ -73,13 +73,13 @@
     <t xml:space="preserve">https://www.digikey.com/products/en?keywords=JK0654219NL</t>
   </si>
   <si>
-    <t xml:space="preserve">TE   282837-2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TE Connectivity   2P Terminal Block</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.com/product-detail/en/te-connectivity-amp-connectors/282837-2/A113320-ND/2187973</t>
+    <t xml:space="preserve">DBParts 20 pc 2-pin 0.1” pitch Terminal Blocks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amazon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.amazon.com/DBParts-20pcs-Terminal-Connector-2-54mm/dp/B07NSJV6NW/ref=sxbs_sxwds-stvp?cv_ct_cx=terminal+block+assortment&amp;keywords=terminal+block+assortment&amp;pd_rd_i=B07NSJV6NW&amp;pd_rd_r=f9187fb7-4ab9-45b4-a445-3bf2b68a1d13&amp;pd_rd_w=WAjjn&amp;pd_rd_wg=olYB9&amp;pf_rd_p=a6d018ad-f20b-46c9-8920-433972c7d9b7&amp;pf_rd_r=PMA44C3EHR468DBRJFP7&amp;psc=1&amp;qid=1581446551&amp;sr=1-3-dd5817a1-1ba7-46c2-8996-f96e7b0f409c</t>
   </si>
   <si>
     <t xml:space="preserve">Adafruit 2772</t>
@@ -271,14 +271,14 @@
   </sheetPr>
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="41.45"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.72"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
@@ -384,22 +384,23 @@
         <v>17</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>1.04</v>
+        <v>6.99</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>73</v>
+        <f aca="false">73/20</f>
+        <v>3.65</v>
       </c>
       <c r="E5" s="2" t="n">
         <f aca="false">C5*D5</f>
-        <v>75.92</v>
+        <v>25.5135</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>19</v>
       </c>
     </row>
@@ -541,7 +542,7 @@
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E14" s="2" t="n">
         <f aca="false">E2+E3+E4+E5+E6+E7+E8+E9+E10</f>
-        <v>107.59</v>
+        <v>57.1835</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Changed footprints for resistors, changed resistor suppliers, and re-routed wires. Need to add mounting holes and clean for ordering.
</commit_message>
<xml_diff>
--- a/LED_Matrix_PCB/BOM.xlsx
+++ b/LED_Matrix_PCB/BOM.xlsx
@@ -91,22 +91,22 @@
     <t xml:space="preserve">https://www.digikey.com/product-detail/en/adafruit-industries-llc/2772/1528-1531-ND/5775537</t>
   </si>
   <si>
-    <t xml:space="preserve">Vishay Dale CRCW2010100RFKEFHP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Solderable size 2010 100 ohm SMD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.com/product-detail/en/vishay-dale/CRCW2010100RFKEFHP/541-100PCT-ND/2222676</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vishay Dale CRCW201010R0FKEF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Solderable size 2010 10 ohm SMD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.com/product-detail/en/vishay-dale/CRCW201010R0FKEF/541-10.0ACCT-ND/1179050</t>
+    <t xml:space="preserve">Stackpole Electronics RSMF2JT330R </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Through Hole 330 ohm 2 watt resistor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/product-detail/en/stackpole-electronics-inc/RSF2JT330R/RSF2JT330RCT-ND/2021796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stackpole Electronics  CF12JT10R0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Through Hole 10 ohm ½ watt Resistor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/product-detail/en/stackpole-electronics-inc/CF12JT10R0/CF12JT10R0CT-ND/1830446</t>
   </si>
   <si>
     <t xml:space="preserve">WIMA FKP0D001000B00JSSD</t>
@@ -272,12 +272,12 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="41.45"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.72"/>
@@ -390,12 +390,12 @@
         <v>6.99</v>
       </c>
       <c r="D5" s="0" t="n">
-        <f aca="false">73/20</f>
-        <v>3.65</v>
+        <f aca="false">_xlfn.CEILING.MATH(73/20)</f>
+        <v>4</v>
       </c>
       <c r="E5" s="2" t="n">
         <f aca="false">C5*D5</f>
-        <v>25.5135</v>
+        <v>27.96</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>18</v>
@@ -436,14 +436,14 @@
         <v>24</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>0.58</v>
+        <v>0.29</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>9</v>
       </c>
       <c r="E7" s="2" t="n">
         <f aca="false">C7*D7</f>
-        <v>5.22</v>
+        <v>2.61</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>9</v>
@@ -460,14 +460,14 @@
         <v>27</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>0.29</v>
+        <v>0.1</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>2</v>
       </c>
       <c r="E8" s="2" t="n">
         <f aca="false">C8*D8</f>
-        <v>0.58</v>
+        <v>0.2</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>9</v>
@@ -542,7 +542,7 @@
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E14" s="2" t="n">
         <f aca="false">E2+E3+E4+E5+E6+E7+E8+E9+E10</f>
-        <v>57.1835</v>
+        <v>56.64</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Changed BOM significantly. Need to swap out screw terminals for 7x7 2-pin headers on schematic. Need to change geometry of the board. Need to change Resistor Footprint. May want to start a new project entirely.
</commit_message>
<xml_diff>
--- a/LED_Matrix_PCB/BOM.xlsx
+++ b/LED_Matrix_PCB/BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -34,6 +34,9 @@
     <t xml:space="preserve">Quantity</t>
   </si>
   <si>
+    <t xml:space="preserve">3X Board Quantity</t>
+  </si>
+  <si>
     <t xml:space="preserve">Total Cost per Board</t>
   </si>
   <si>
@@ -64,22 +67,34 @@
     <t xml:space="preserve">https://www.digikey.com/product-detail/en/bourns-inc/CDSOT23-SM712/CDSOT23-SM712CT-ND/1630607</t>
   </si>
   <si>
-    <t xml:space="preserve">Amphenol ICC 54601-908WPLF  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RJ-45 Mountable connector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.com/products/en?keywords=JK0654219NL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DBParts 20 pc 2-pin 0.1” pitch Terminal Blocks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amazon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.amazon.com/DBParts-20pcs-Terminal-Connector-2-54mm/dp/B07NSJV6NW/ref=sxbs_sxwds-stvp?cv_ct_cx=terminal+block+assortment&amp;keywords=terminal+block+assortment&amp;pd_rd_i=B07NSJV6NW&amp;pd_rd_r=f9187fb7-4ab9-45b4-a445-3bf2b68a1d13&amp;pd_rd_w=WAjjn&amp;pd_rd_wg=olYB9&amp;pf_rd_p=a6d018ad-f20b-46c9-8920-433972c7d9b7&amp;pf_rd_r=PMA44C3EHR468DBRJFP7&amp;psc=1&amp;qid=1581446551&amp;sr=1-3-dd5817a1-1ba7-46c2-8996-f96e7b0f409c</t>
+    <t xml:space="preserve">Adam Tech MTS-02 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CONN HOUSING 2POS 2.54MM </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digi-Key</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/product-detail/en/adam-tech/MTS-02/2057-MTS-02-ND/9830694</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TE Connectivity 640456-2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONN HEADER VERT 2POS 2.54MM </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/product-detail/en/te-connectivity-amp-connectors/640456-2/A1921-ND/109003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On Semiconductor NTD3055L104-1G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">200 mA 2Vgss Mosfet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/product-detail/en/on-semiconductor/NTD3055L104-1G/NTD3055L104-1GOS-ND/1484764</t>
   </si>
   <si>
     <t xml:space="preserve">Adafruit 2772</t>
@@ -91,31 +106,22 @@
     <t xml:space="preserve">https://www.digikey.com/product-detail/en/adafruit-industries-llc/2772/1528-1531-ND/5775537</t>
   </si>
   <si>
-    <t xml:space="preserve">Stackpole Electronics RSMF2JT330R </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Through Hole 330 ohm 2 watt resistor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.com/product-detail/en/stackpole-electronics-inc/RSF2JT330R/RSF2JT330RCT-ND/2021796</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stackpole Electronics  CF12JT10R0 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Through Hole 10 ohm ½ watt Resistor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.com/product-detail/en/stackpole-electronics-inc/CF12JT10R0/CF12JT10R0CT-ND/1830446</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WIMA FKP0D001000B00JSSD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Radial 100 pF Film Cap </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.com/product-detail/en/wima/FKP0D001000B00JSSD/1928-1039-ND/9370034</t>
+    <t xml:space="preserve">Stackpole Electronics RSMF2JT300R </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Through Hole 300 ohm 2 watt resistor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/product-detail/en/stackpole-electronics-inc/RSMF2JT300R/RSMF2JT300RCT-ND/2021864</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stackpole Electronics  CF14JT10K0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Through Hole 10k ohm ½ watt Resistor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/product-detail/en/stackpole-electronics-inc/CF14JT10K0/CF14JT10K0CT-ND/1830374</t>
   </si>
   <si>
     <t xml:space="preserve">Nichicon UVK2GR47MED1TD </t>
@@ -125,6 +131,12 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.digikey.com/product-detail/en/nichicon/UVK2GR47MED1TD/493-12648-3-ND/4328849</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OFNMY LED Kit 500 pc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.amazon.com/OFNMY-5mm-Diode-Lights-Assortment/dp/B082VWC211/ref=sr_1_1?keywords=LED+white+prototyping&amp;qid=1582384296&amp;sr=8-1</t>
   </si>
   <si>
     <t xml:space="preserve">*Discount prices are available for the</t>
@@ -231,7 +243,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -245,6 +257,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -269,19 +289,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="41.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="47.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.85"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.72"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="19.72"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -306,13 +326,16 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>2.65</v>
@@ -320,23 +343,27 @@
       <c r="D2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="2" t="n">
+      <c r="E2" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(3*D2)</f>
+        <v>3</v>
+      </c>
+      <c r="F2" s="2" t="n">
         <f aca="false">C2*D2</f>
         <v>2.65</v>
       </c>
-      <c r="F2" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="0" t="s">
         <v>10</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>1.53</v>
@@ -344,168 +371,195 @@
       <c r="D3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E3" s="2" t="n">
+      <c r="E3" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(3*D3)</f>
+        <v>3</v>
+      </c>
+      <c r="F3" s="2" t="n">
         <f aca="false">C3*D3</f>
         <v>1.53</v>
       </c>
-      <c r="F3" s="0" t="s">
-        <v>9</v>
-      </c>
       <c r="G3" s="0" t="s">
-        <v>13</v>
+        <v>10</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>0.49</v>
+        <v>0.1</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E4" s="2" t="n">
+        <v>52</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(3*D4)</f>
+        <v>156</v>
+      </c>
+      <c r="F4" s="2" t="n">
         <f aca="false">C4*D4</f>
-        <v>0.98</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>16</v>
+        <v>5.2</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>52</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(3*D5)</f>
+        <v>156</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <f aca="false">C5*D5</f>
+        <v>5.72</v>
+      </c>
+      <c r="G5" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="2" t="n">
-        <v>6.99</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <f aca="false">_xlfn.CEILING.MATH(73/20)</f>
-        <v>4</v>
-      </c>
-      <c r="E5" s="2" t="n">
-        <f aca="false">C5*D5</f>
-        <v>27.96</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>20</v>
+      <c r="H5" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>19.95</v>
+        <v>0.62</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E6" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(3*D6)</f>
+        <v>42</v>
+      </c>
+      <c r="F6" s="2" t="n">
         <f aca="false">C6*D6</f>
-        <v>19.95</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>22</v>
+        <v>8.68</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>0.29</v>
+        <v>19.95</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="E7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(3*D7)</f>
+        <v>3</v>
+      </c>
+      <c r="F7" s="2" t="n">
         <f aca="false">C7*D7</f>
-        <v>2.61</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>25</v>
+        <v>19.95</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>0.1</v>
+        <v>0.28</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E8" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(3*D8)</f>
+        <v>84</v>
+      </c>
+      <c r="F8" s="2" t="n">
         <f aca="false">C8*D8</f>
-        <v>0.2</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>28</v>
+        <v>7.84</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>0.7</v>
+        <v>0.1</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E9" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(3*D9)</f>
+        <v>42</v>
+      </c>
+      <c r="F9" s="2" t="n">
         <f aca="false">C9*D9</f>
-        <v>0.7</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>31</v>
+        <v>1.4</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>0.06</v>
@@ -513,58 +567,90 @@
       <c r="D10" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E10" s="2" t="n">
+      <c r="E10" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(3*D10)</f>
+        <v>3</v>
+      </c>
+      <c r="F10" s="2" t="n">
         <f aca="false">C10*D10</f>
         <v>0.06</v>
       </c>
-      <c r="F10" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>34</v>
+      <c r="G10" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="G11" s="3"/>
+      <c r="A11" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>9.99</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <f aca="false">49/100</f>
+        <v>0.49</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(3*D11)</f>
+        <v>2</v>
+      </c>
+      <c r="F11" s="2" t="n">
+        <f aca="false">C11*D11</f>
+        <v>4.8951</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="G12" s="3"/>
+      <c r="F12" s="2"/>
+      <c r="H12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E13" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="C13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="H13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E14" s="2" t="n">
-        <f aca="false">E2+E3+E4+E5+E6+E7+E8+E9+E10</f>
-        <v>56.64</v>
+      <c r="F14" s="6" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E15" s="0" t="s">
-        <v>35</v>
+      <c r="F15" s="2" t="n">
+        <f aca="false">F2+F3+F4+F5+F6+F7+F8+F9+F10+F11</f>
+        <v>57.9251</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E16" s="0" t="s">
-        <v>36</v>
+      <c r="F16" s="0" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E17" s="0" t="s">
-        <v>37</v>
+      <c r="F17" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F18" s="0" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" display="https://www.digikey.com/product-detail/en/texas-instruments/SN65HVD72DR/296-39179-1-ND/5143186"/>
-    <hyperlink ref="G4" r:id="rId2" display="https://www.digikey.com/products/en?keywords=JK0654219NL"/>
-    <hyperlink ref="G6" r:id="rId3" display="https://www.digikey.com/product-detail/en/adafruit-industries-llc/2772/1528-1531-ND/5775537"/>
+    <hyperlink ref="H2" r:id="rId1" display="https://www.digikey.com/product-detail/en/texas-instruments/SN65HVD72DR/296-39179-1-ND/5143186"/>
+    <hyperlink ref="H7" r:id="rId2" display="https://www.digikey.com/product-detail/en/adafruit-industries-llc/2772/1528-1531-ND/5775537"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Forgot to close files before pushing.
</commit_message>
<xml_diff>
--- a/LED_Matrix_PCB/BOM.xlsx
+++ b/LED_Matrix_PCB/BOM.xlsx
@@ -88,13 +88,13 @@
     <t xml:space="preserve">https://www.digikey.com/product-detail/en/te-connectivity-amp-connectors/640456-2/A1921-ND/109003</t>
   </si>
   <si>
-    <t xml:space="preserve">On Semiconductor NTD3055L104-1G</t>
+    <t xml:space="preserve">On Semiconductor 2N7000</t>
   </si>
   <si>
     <t xml:space="preserve">200 mA 2Vgss Mosfet</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.digikey.com/product-detail/en/on-semiconductor/NTD3055L104-1G/NTD3055L104-1GOS-ND/1484764</t>
+    <t xml:space="preserve">https://www.digikey.com/product-detail/en/on-semiconductor/2N7000/2N7000FS-ND/244278</t>
   </si>
   <si>
     <t xml:space="preserve">Adafruit 2772</t>
@@ -292,7 +292,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -450,7 +450,7 @@
         <v>23</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>0.62</v>
+        <v>0.32</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>14</v>
@@ -461,7 +461,7 @@
       </c>
       <c r="F6" s="2" t="n">
         <f aca="false">C6*D6</f>
-        <v>8.68</v>
+        <v>4.48</v>
       </c>
       <c r="G6" s="0" t="s">
         <v>10</v>
@@ -629,7 +629,7 @@
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F15" s="2" t="n">
         <f aca="false">F2+F3+F4+F5+F6+F7+F8+F9+F10+F11</f>
-        <v>57.9251</v>
+        <v>53.7251</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added a pull down resistor and re-routed. Also, updated BOM.
</commit_message>
<xml_diff>
--- a/LED_Matrix_PCB/BOM.xlsx
+++ b/LED_Matrix_PCB/BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -118,19 +118,28 @@
     <t xml:space="preserve">Stackpole Electronics  CF12JT10R0 </t>
   </si>
   <si>
-    <t xml:space="preserve">Through Hole 10 ohm ½ watt Resistor</t>
+    <t xml:space="preserve">Through Hole 10 ohm ¼ watt Resistor</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.digikey.com/product-detail/en/stackpole-electronics-inc/CF12JT10R0/CF12JT10R0CT-ND/1830446</t>
   </si>
   <si>
-    <t xml:space="preserve">Stackpole Electronics  CF14JT10K0 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Through Hole 10k ohm ½ watt Resistor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.com/product-detail/en/stackpole-electronics-inc/CF14JT10K0/CF14JT10K0CT-ND/1830374</t>
+    <t xml:space="preserve">Stackpole Electronics  CF14JT100R </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Through Hole 100 ohm ¼ watt Resistor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/product-detail/en/stackpole-electronics-inc/CF14JT100R/CF14JT100RCT-ND/1830327</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stackpole Electronics  CF18JT3K00 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Through Hole 3k ohm 1/4 watt Resistor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/product-detail/en/stackpole-electronics-inc/CF18JT3K00/CF18JT3K00CT-ND/2022753</t>
   </si>
   <si>
     <t xml:space="preserve">Nichicon UVK2GR47MED1TD </t>
@@ -298,10 +307,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -599,18 +608,18 @@
         <v>38</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>0.06</v>
+        <v>0.1</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="E11" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(3*D11)</f>
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="F11" s="2" t="n">
         <f aca="false">C11*D11</f>
-        <v>0.06</v>
+        <v>1.4</v>
       </c>
       <c r="G11" s="0" t="s">
         <v>10</v>
@@ -624,34 +633,57 @@
         <v>40</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C12" s="2" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(3*D12)</f>
+        <v>3</v>
+      </c>
+      <c r="F12" s="2" t="n">
+        <f aca="false">C12*D12</f>
+        <v>0.06</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="2" t="n">
         <v>9.99</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="D13" s="0" t="n">
         <f aca="false">49/100</f>
         <v>0.49</v>
       </c>
-      <c r="E12" s="0" t="n">
-        <f aca="false">_xlfn.CEILING.MATH(3*D12)</f>
+      <c r="E13" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(3*D13)</f>
         <v>2</v>
       </c>
-      <c r="F12" s="2" t="n">
-        <f aca="false">C12*D12</f>
+      <c r="F13" s="2" t="n">
+        <f aca="false">C13*D13</f>
         <v>4.8951</v>
       </c>
-      <c r="G12" s="0" t="s">
+      <c r="G13" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="H12" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="H13" s="3"/>
+      <c r="H13" s="3" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="2"/>
@@ -659,29 +691,34 @@
       <c r="H14" s="3"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F15" s="6" t="s">
+      <c r="C15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="H15" s="3"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F16" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F16" s="2" t="n">
-        <f aca="false">F2+F3+F4+F5+F6+F7+F8+F10+F11+F12</f>
-        <v>47.8451</v>
-      </c>
-    </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F17" s="0" t="s">
-        <v>42</v>
+      <c r="F17" s="2" t="n">
+        <f aca="false">F2+F3+F4+F5+F6+F7+F8+F10++F11+F12+F13</f>
+        <v>49.2451</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F18" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F19" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F20" s="0" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>